<commit_message>
Reformatted author page, added external labels
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99033042-9E2A-D848-96A1-6584212425D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218D4EEC-798B-8646-AD4E-15EBBA10C0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Column_list" sheetId="1" r:id="rId1"/>
+    <sheet name="Table_list" sheetId="2" r:id="rId2"/>
+    <sheet name="Translatable_Site_labels" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="175">
   <si>
     <t>#</t>
   </si>
@@ -44,6 +46,9 @@
     <t>Label</t>
   </si>
   <si>
+    <t>Component</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -387,6 +392,177 @@
   </si>
   <si>
     <t>Publisher name</t>
+  </si>
+  <si>
+    <t>TEXT_ID</t>
+  </si>
+  <si>
+    <t>TEXT_TITLE</t>
+  </si>
+  <si>
+    <t>TEXT_AUTHOR</t>
+  </si>
+  <si>
+    <t>TEXT_TYPE</t>
+  </si>
+  <si>
+    <t>TEXT_GENRE</t>
+  </si>
+  <si>
+    <t>TEXT_LANGUAGE</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_DATE</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_YEAR</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_MONTH</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_DAY</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_PUBLISHER</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_TYPE</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_LENGTH</t>
+  </si>
+  <si>
+    <t>TEXT_WRITING_START</t>
+  </si>
+  <si>
+    <t>TEXT_WRITING_END</t>
+  </si>
+  <si>
+    <t>Table Name</t>
+  </si>
+  <si>
+    <t>Table Description</t>
+  </si>
+  <si>
+    <t>AUTHOR</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>AUTHOR_NAMES</t>
+  </si>
+  <si>
+    <t>AUTHOR_BIOGRAPHIES</t>
+  </si>
+  <si>
+    <t>AUTHOR_INFLUENCES</t>
+  </si>
+  <si>
+    <t>AUTHOR_INFLUENCED</t>
+  </si>
+  <si>
+    <t>AUTHOR_SOURCES</t>
+  </si>
+  <si>
+    <t>AUTHOR_OCCUPATIONS</t>
+  </si>
+  <si>
+    <t>TEXT_AUTHORS</t>
+  </si>
+  <si>
+    <t>TEXT_GENRES</t>
+  </si>
+  <si>
+    <t>EDITION</t>
+  </si>
+  <si>
+    <t>EDITION_PARTIES</t>
+  </si>
+  <si>
+    <t>Translated</t>
+  </si>
+  <si>
+    <t>aka.</t>
+  </si>
+  <si>
+    <t>Born:</t>
+  </si>
+  <si>
+    <t>Nationality:</t>
+  </si>
+  <si>
+    <t>Floruit:</t>
+  </si>
+  <si>
+    <t>Occupation:</t>
+  </si>
+  <si>
+    <t>(wikipedia)</t>
+  </si>
+  <si>
+    <t>Influences:</t>
+  </si>
+  <si>
+    <t>Influenced:</t>
+  </si>
+  <si>
+    <t>List of known works</t>
+  </si>
+  <si>
+    <t>Add works:</t>
+  </si>
+  <si>
+    <t>Label Name</t>
+  </si>
+  <si>
+    <t>aka</t>
+  </si>
+  <si>
+    <t>born</t>
+  </si>
+  <si>
+    <t>died</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>floruit</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>wiki</t>
+  </si>
+  <si>
+    <t>influence</t>
+  </si>
+  <si>
+    <t>influenced</t>
+  </si>
+  <si>
+    <t>works</t>
+  </si>
+  <si>
+    <t>add_works</t>
+  </si>
+  <si>
+    <t>Died:</t>
+  </si>
+  <si>
+    <t>not specified</t>
+  </si>
+  <si>
+    <t>unspecified</t>
+  </si>
+  <si>
+    <t>also known as..</t>
+  </si>
+  <si>
+    <t>other_occupations</t>
   </si>
 </sst>
 </file>
@@ -847,18 +1023,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35313EE5-8BCE-A449-9C2B-DB968751C49B}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E45" sqref="E45"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="1" customWidth="1"/>
     <col min="4" max="4" width="52" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
@@ -872,16 +1048,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -889,19 +1065,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -909,19 +1085,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -929,19 +1105,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -949,19 +1125,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -969,19 +1145,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -989,19 +1165,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1009,19 +1185,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1029,19 +1205,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1049,19 +1225,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1069,19 +1245,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1089,19 +1265,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1109,19 +1285,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1129,19 +1305,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1149,19 +1325,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1169,19 +1345,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1189,19 +1365,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1209,19 +1385,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1229,19 +1405,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1249,19 +1425,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1269,19 +1445,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1289,19 +1465,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1309,19 +1485,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1329,19 +1505,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1349,19 +1525,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1369,19 +1545,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1389,257 +1565,359 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
       <c r="B28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+      <c r="E44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1648,4 +1926,325 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101CA093-5802-DD4F-8107-ADDDA1A2FFE1}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f t="shared" ref="E2:E14" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
+        <v>aka : 'aka.',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>born : 'Born:',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>died : 'Died:',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>nationality : 'Nationality:',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>floruit : 'Floruit:',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>occupation : 'Occupation:',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>other_occupations : 'also known as..',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>wiki : '(wikipedia)',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>influence : 'Influences:',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>influenced : 'Influenced:',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>works : 'List of known works',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>add_works : 'Add works:',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>unspecified : 'not specified',</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added component for author & text list elements, other simplifications
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F19D49-3337-F845-85A0-8AEB2102CD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B5CFB1-00E8-E242-AB15-82BE0AF5DAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Column_list" sheetId="1" r:id="rId1"/>
     <sheet name="Table_list" sheetId="2" r:id="rId2"/>
     <sheet name="Translatable_Site_labels" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="187">
   <si>
     <t>#</t>
   </si>
@@ -487,15 +487,6 @@
     <t>aka.</t>
   </si>
   <si>
-    <t>Nationality:</t>
-  </si>
-  <si>
-    <t>Floruit:</t>
-  </si>
-  <si>
-    <t>Occupation:</t>
-  </si>
-  <si>
     <t>(wikipedia)</t>
   </si>
   <si>
@@ -563,6 +554,51 @@
   </si>
   <si>
     <t>Died</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_LENGTH_TYPE</t>
+  </si>
+  <si>
+    <t>author_name</t>
+  </si>
+  <si>
+    <t>original_language</t>
+  </si>
+  <si>
+    <t>Original language(s)</t>
+  </si>
+  <si>
+    <t>Original publication date</t>
+  </si>
+  <si>
+    <t>original_publication_date</t>
+  </si>
+  <si>
+    <t>Original publisher</t>
+  </si>
+  <si>
+    <t>original_publisher_name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>original_publication_type</t>
+  </si>
+  <si>
+    <t>original_publication_length</t>
+  </si>
+  <si>
+    <t>Writing period</t>
+  </si>
+  <si>
+    <t>writing_period</t>
   </si>
 </sst>
 </file>
@@ -636,7 +672,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="3" tint="-0.249977111117893"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -692,7 +728,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="3" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
@@ -710,22 +746,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C92C06A-FB8E-9D44-AF23-A294384A6499}" name="Table1" displayName="Table1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C92C06A-FB8E-9D44-AF23-A294384A6499}" name="Table1" displayName="Table1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F45" xr:uid="{2C92C06A-FB8E-9D44-AF23-A294384A6499}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A5E7B0C6-2074-3F43-82F5-8187B0E8F44E}" name="#" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{266CDBC5-C85E-8B4C-8E05-3898F7A33CD4}" name="Label" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C52FD609-C89F-3942-896D-6DC79FC67526}" name="SQL name" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{27DED3B4-AC6F-734A-8500-9C1E45380767}" name="Description" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{8F972DE9-9931-1C42-9EE0-B8076AF4B907}" name="Datatype" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{AD8E2AEE-C3DE-594D-9D4A-21338761046F}" name="Table" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A5E7B0C6-2074-3F43-82F5-8187B0E8F44E}" name="#" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{266CDBC5-C85E-8B4C-8E05-3898F7A33CD4}" name="Label" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C52FD609-C89F-3942-896D-6DC79FC67526}" name="SQL name" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{27DED3B4-AC6F-734A-8500-9C1E45380767}" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{8F972DE9-9931-1C42-9EE0-B8076AF4B907}" name="Datatype" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{AD8E2AEE-C3DE-594D-9D4A-21338761046F}" name="Table" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1013,7 +1049,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1024,17 +1060,17 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="52" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
@@ -1868,7 +1904,7 @@
         <v>102</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>130</v>
+        <v>173</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>103</v>
@@ -2021,10 +2057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2037,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2051,7 +2087,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>148</v>
@@ -2060,16 +2096,16 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E14" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
+        <f t="shared" ref="E2:E22" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
         <v>aka : 'aka.',</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -2081,10 +2117,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
@@ -2096,55 +2132,55 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>nationality : 'Nationality:',</v>
+        <v>nationality : 'Nationality',</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>floruit : 'Floruit:',</v>
+        <v>floruit : 'Floruit',</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>occupation : 'Occupation:',</v>
+        <v>occupation : 'Occupation',</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
@@ -2156,10 +2192,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
@@ -2171,10 +2207,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>27</v>
@@ -2186,10 +2222,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>27</v>
@@ -2201,10 +2237,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -2216,10 +2252,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>27</v>
@@ -2231,10 +2267,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>27</v>
@@ -2242,6 +2278,126 @@
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>unspecified : 'not specified',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>aka : 'aka.',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>author_name : 'Author',</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>original_language : 'Original language(s)',</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>original_publication_date : 'Original publication date',</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>original_publisher_name : 'Original publisher',</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>original_publication_type : 'Type',</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>original_publication_length : 'Length',</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>writing_period : 'Writing period',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added basic edition page
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B675ED2C-9860-A243-BF82-856F46EB5A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B42647-8EA2-9342-B87F-120BE961A0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Column_list" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="239">
   <si>
     <t>#</t>
   </si>
@@ -707,6 +707,54 @@
   </si>
   <si>
     <t>Type of binding of the edition: "hardcover, paperback, ebook, etc"</t>
+  </si>
+  <si>
+    <t>edition_title</t>
+  </si>
+  <si>
+    <t>edition_editors</t>
+  </si>
+  <si>
+    <t>editors</t>
+  </si>
+  <si>
+    <t>Editors</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>edition_language</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>original_title</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>binding</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>publication</t>
+  </si>
+  <si>
+    <t>Original Title</t>
+  </si>
+  <si>
+    <t>Published</t>
+  </si>
+  <si>
+    <t>length</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35313EE5-8BCE-A449-9C2B-DB968751C49B}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2405,10 +2453,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2444,7 +2492,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E24" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
+        <f t="shared" ref="E2:E38" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
         <v>aka : 'aka.',</v>
       </c>
     </row>
@@ -2776,6 +2824,216 @@
       <c r="E24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>unspecified : 'not specified',</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>edition_title : 'Title',</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>edition_editors : 'Editors',</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>edition_language : 'Language',</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>isbn : 'ISBN',</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>author : 'Author',</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>original_title : 'Original Title',</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>language : 'Language',</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>editors : 'Editors',</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>isbn : 'ISBN',</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>publisher : 'Publisher',</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>binding : 'Binding',</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pages : 'pages',</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>publication : 'Published',</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>length : 'Length',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added basic import functionality. Adjusted header formatting
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B42647-8EA2-9342-B87F-120BE961A0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BDA50F-3728-F243-871B-47820E22A175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="247">
   <si>
     <t>#</t>
   </si>
@@ -755,6 +755,30 @@
   </si>
   <si>
     <t>length</t>
+  </si>
+  <si>
+    <t>ISBN10/13</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>import_header</t>
+  </si>
+  <si>
+    <t>Data Import</t>
+  </si>
+  <si>
+    <t>import_type</t>
+  </si>
+  <si>
+    <t>import_type_select</t>
+  </si>
+  <si>
+    <t>Select list type</t>
+  </si>
+  <si>
+    <t>Please select import type</t>
   </si>
 </sst>
 </file>
@@ -2453,10 +2477,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2492,7 +2516,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E38" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
+        <f t="shared" ref="E2:E41" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
         <v>aka : 'aka.',</v>
       </c>
     </row>
@@ -2951,14 +2975,14 @@
         <v>229</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>195</v>
+        <v>239</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>189</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>isbn : 'ISBN',</v>
+        <v>isbn : 'ISBN10/13',</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
@@ -3034,6 +3058,51 @@
       <c r="E38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>length : 'Length',</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_header : 'Data Import',</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_type : 'Please select import type',</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_type_select : 'Select list type',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added baseline functions to import
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BDA50F-3728-F243-871B-47820E22A175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD3B309-579D-C847-8C6B-0DA789FDFCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="255">
   <si>
     <t>#</t>
   </si>
@@ -775,10 +775,34 @@
     <t>import_type_select</t>
   </si>
   <si>
-    <t>Select list type</t>
-  </si>
-  <si>
     <t>Please select import type</t>
+  </si>
+  <si>
+    <t>Import type</t>
+  </si>
+  <si>
+    <t>import_preview_header</t>
+  </si>
+  <si>
+    <t>Preview</t>
+  </si>
+  <si>
+    <t>import_upload_data</t>
+  </si>
+  <si>
+    <t>Upload data</t>
+  </si>
+  <si>
+    <t>import_preview_label</t>
+  </si>
+  <si>
+    <t>Please change column names using the dropdowns</t>
+  </si>
+  <si>
+    <t>import_push_data</t>
+  </si>
+  <si>
+    <t>Push data to database</t>
   </si>
 </sst>
 </file>
@@ -2477,10 +2501,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2516,7 +2540,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E41" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
+        <f t="shared" ref="E2:E45" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
         <v>aka : 'aka.',</v>
       </c>
     </row>
@@ -3080,7 +3104,7 @@
         <v>243</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>240</v>
@@ -3095,14 +3119,74 @@
         <v>244</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>240</v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_type_select : 'Select list type',</v>
+        <v>import_type_select : 'Import type',</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_preview_header : 'Preview',</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_upload_data : 'Upload data',</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_preview_label : 'Please change column names using the dropdowns',</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_push_data : 'Push data to database',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added API and moved dataformatting to backend (Python)
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD3B309-579D-C847-8C6B-0DA789FDFCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577D9CA4-EDA1-D143-8346-D30426CA39FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
@@ -1264,10 +1264,10 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2504,7 +2504,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added edit page for texts
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577D9CA4-EDA1-D143-8346-D30426CA39FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C41014C-4C69-E742-9D80-96FCC88CCBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="284">
   <si>
     <t>#</t>
   </si>
@@ -481,9 +481,6 @@
     <t>EDITION_PARTIES</t>
   </si>
   <si>
-    <t>Translated</t>
-  </si>
-  <si>
     <t>aka.</t>
   </si>
   <si>
@@ -757,9 +754,6 @@
     <t>length</t>
   </si>
   <si>
-    <t>ISBN10/13</t>
-  </si>
-  <si>
     <t>Import</t>
   </si>
   <si>
@@ -803,6 +797,99 @@
   </si>
   <si>
     <t>Push data to database</t>
+  </si>
+  <si>
+    <t>import_refresh</t>
+  </si>
+  <si>
+    <t>Refresh</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>import_type_authors</t>
+  </si>
+  <si>
+    <t>import_type_texts</t>
+  </si>
+  <si>
+    <t>import_type_editions</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Texts</t>
+  </si>
+  <si>
+    <t>import_error</t>
+  </si>
+  <si>
+    <t>Data has not been imported or the data imported is empty</t>
+  </si>
+  <si>
+    <t>import_databtn</t>
+  </si>
+  <si>
+    <t>latest_editsbtn</t>
+  </si>
+  <si>
+    <t>admin_header</t>
+  </si>
+  <si>
+    <t>Imported data</t>
+  </si>
+  <si>
+    <t>Latest edits</t>
+  </si>
+  <si>
+    <t>edit_country_birth_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (city, country) of birth</t>
+  </si>
+  <si>
+    <t>submit_edits</t>
+  </si>
+  <si>
+    <t>Submit Edits</t>
+  </si>
+  <si>
+    <t>editBtn</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>exitEditBtn</t>
+  </si>
+  <si>
+    <t>Stop Editing</t>
+  </si>
+  <si>
+    <t>edit_country_death_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (city, country) of death</t>
+  </si>
+  <si>
+    <t>const labels = {</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>export default labels;</t>
+  </si>
+  <si>
+    <t>Author/Text/Editions</t>
+  </si>
+  <si>
+    <t>Undo all changes</t>
+  </si>
+  <si>
+    <t>undoEditBtn</t>
   </si>
 </sst>
 </file>
@@ -2108,7 +2195,7 @@
         <v>102</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>103</v>
@@ -2165,19 +2252,19 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2185,19 +2272,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2217,7 +2304,7 @@
         <v>65</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2225,19 +2312,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2245,19 +2332,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2265,19 +2352,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2285,19 +2372,19 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>69</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2305,19 +2392,19 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2325,19 +2412,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2345,19 +2432,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2365,19 +2452,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2385,19 +2472,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2501,10 +2588,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2517,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2526,7 +2613,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>147</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2534,14 +2621,14 @@
         <v>155</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E45" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
-        <v>aka : 'aka.',</v>
+        <f t="shared" ref="E2:E56" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
+        <v>born : 'Born',</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2556,7 +2643,7 @@
       </c>
       <c r="E3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>born : 'Born',</v>
+        <v>died : 'Died',</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2564,14 +2651,14 @@
         <v>157</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>died : 'Died',</v>
+        <v>nationality : 'Nationality',</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2579,14 +2666,14 @@
         <v>158</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>nationality : 'Nationality',</v>
+        <v>floruit : 'Floruit',</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2594,44 +2681,44 @@
         <v>159</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>170</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>floruit : 'Floruit',</v>
+        <v>occupation : 'Occupation',</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>occupation : 'Occupation',</v>
+        <v>other_occupations : 'also known as ',</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>other_occupations : 'also known as ',</v>
+        <v>wiki : '(wikipedia)',</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2646,7 +2733,7 @@
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>wiki : '(wikipedia)',</v>
+        <v>influence : 'Influences:',</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2661,7 +2748,7 @@
       </c>
       <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>influence : 'Influences:',</v>
+        <v>influenced : 'Influenced:',</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2676,7 +2763,7 @@
       </c>
       <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>influenced : 'Influenced:',</v>
+        <v>works : 'List of known works',</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2691,502 +2778,677 @@
       </c>
       <c r="E12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>works : 'List of known works',</v>
+        <v>add_works : 'Add works:',</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>add_works : 'Add works:',</v>
+        <v>unspecified : 'not specified',</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>167</v>
+        <v>270</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>166</v>
+        <v>271</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>unspecified : 'not specified',</v>
+        <v>submit_edits : 'Submit Edits',</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>148</v>
+        <v>269</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>aka : 'aka.',</v>
+        <f t="shared" ref="E15:E16" si="1">_xlfn.CONCAT("",B15," : '",C15,"',")</f>
+        <v>edit_country_birth_description : ' (city, country) of birth',</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>173</v>
+        <v>276</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>277</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>author_name : 'Author',</v>
+        <f t="shared" si="1"/>
+        <v>edit_country_death_description : ' (city, country) of death',</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>187</v>
+        <v>273</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_language : 'Original Language(s)',</v>
+        <v>editBtn : 'Edit',</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>175</v>
+        <v>274</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>185</v>
+        <v>275</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_publication_date : 'Original Publication',</v>
+        <v>exitEditBtn : 'Stop Editing',</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_publisher_name : 'Original Publisher',</v>
+        <v>aka : 'aka.',</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_publication_type : 'Type',</v>
+        <v>author_name : 'Author',</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_publication_length : 'Length',</v>
+        <v>original_language : 'Original Language(s)',</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>writing_period : 'Writing period',</v>
+        <v>original_publication_date : 'Original Publication',</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>editions : 'Editions',</v>
+        <v>original_publisher_name : 'Original Publisher',</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>unspecified : 'not specified',</v>
+        <v>original_publication_type : 'Type',</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>edition_title : 'Title',</v>
+        <v>original_publication_length : 'Length',</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>226</v>
+        <v>180</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>edition_editors : 'Editors',</v>
+        <v>writing_period : 'Writing period',</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>228</v>
+        <v>183</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>edition_language : 'Language',</v>
+        <v>editions : 'Editions',</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>isbn : 'ISBN',</v>
+        <v>edition_title : 'Title',</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>225</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>189</v>
+        <v>84</v>
       </c>
       <c r="E29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>author : 'Author',</v>
+        <v>edition_editors : 'Editors',</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>189</v>
+        <v>84</v>
       </c>
       <c r="E30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_title : 'Original Title',</v>
+        <v>edition_language : 'Language',</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>189</v>
+        <v>84</v>
       </c>
       <c r="E31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>language : 'Language',</v>
+        <v>isbn : 'ISBN',</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>226</v>
+        <v>27</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>editors : 'Editors',</v>
+        <v>author : 'Author',</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>isbn : 'ISBN10/13',</v>
+        <v>original_title : 'Original Title',</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>publisher : 'Publisher',</v>
+        <v>language : 'Language',</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>binding : 'Binding',</v>
+        <v>editors : 'Editors',</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>234</v>
+        <v>192</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>pages : 'pages',</v>
+        <v>publisher : 'Publisher',</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>publication : 'Published',</v>
+        <v>binding : 'Binding',</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>178</v>
+        <v>233</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>length : 'Length',</v>
+        <v>pages : 'pages',</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>240</v>
+        <v>188</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_header : 'Data Import',</v>
+        <v>publication : 'Published',</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>245</v>
+        <v>177</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>240</v>
+        <v>188</v>
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_type : 'Please select import type',</v>
+        <v>length : 'Length',</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_type_select : 'Import type',</v>
+        <v>import_header : 'Data Import',</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E42" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_preview_header : 'Preview',</v>
+        <v>import_type : 'Please select import type',</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E43" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_upload_data : 'Upload data',</v>
+        <v>import_type_select : 'Import type',</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_preview_label : 'Please change column names using the dropdowns',</v>
+        <v>import_preview_header : 'Preview',</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_upload_data : 'Upload data',</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_preview_label : 'Please change column names using the dropdowns',</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_push_data : 'Push data to database',</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>import_push_data : 'Push data to database',</v>
+      <c r="D48" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_refresh : 'Refresh',</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_type_authors : 'Authors',</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_type_texts : 'Texts',</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_type_editions : 'Editions',</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_error : 'Data has not been imported or the data imported is empty',</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>import_databtn : 'Imported data',</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>latest_editsbtn : 'Latest edits',</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>admin_header : 'Admin',</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>undoEditBtn : 'Undo all changes',</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E59" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Div minor changes, change of import approval to post
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C41014C-4C69-E742-9D80-96FCC88CCBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A207403D-0290-2A42-9A15-6EA4CAAF6FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="291">
   <si>
     <t>#</t>
   </si>
@@ -890,6 +890,27 @@
   </si>
   <si>
     <t>undoEditBtn</t>
+  </si>
+  <si>
+    <t>Site Header</t>
+  </si>
+  <si>
+    <t>homeBtn</t>
+  </si>
+  <si>
+    <t>detailedSearchBtn</t>
+  </si>
+  <si>
+    <t>importDataBtn</t>
+  </si>
+  <si>
+    <t>adminBtn</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Detailed Search</t>
   </si>
 </sst>
 </file>
@@ -2588,10 +2609,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2627,7 +2648,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E56" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
+        <f t="shared" ref="E2:E60" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
         <v>born : 'Born',</v>
       </c>
     </row>
@@ -3442,12 +3463,72 @@
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E57" s="1" t="s">
+      <c r="B57" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>homeBtn : 'Home',</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>detailedSearchBtn : 'Detailed Search',</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>importDataBtn : 'Import',</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>adminBtn : 'Admin',</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E61" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E59" s="1" t="s">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E63" s="1" t="s">
         <v>280</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Various adjustments. Addition of changing author in texts page
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A207403D-0290-2A42-9A15-6EA4CAAF6FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347951D7-0373-E64B-8BC9-3F61149F35A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="293">
   <si>
     <t>#</t>
   </si>
@@ -911,6 +911,12 @@
   </si>
   <si>
     <t>Detailed Search</t>
+  </si>
+  <si>
+    <t>No known works</t>
+  </si>
+  <si>
+    <t>worksUnknown</t>
   </si>
 </sst>
 </file>
@@ -2609,10 +2615,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E1" sqref="E1:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2648,7 +2654,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E60" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
+        <f t="shared" ref="E2:E61" si="0">_xlfn.CONCAT("",B2," : '",C2,"',")</f>
         <v>born : 'Born',</v>
       </c>
     </row>
@@ -2767,9 +2773,8 @@
       <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>influenced : 'Influenced:',</v>
+      <c r="E10" s="1" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2894,641 +2899,656 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>154</v>
+        <v>292</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>147</v>
+        <v>291</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>aka : 'aka.',</v>
+        <v>worksUnknown : 'No known works',</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>147</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>author_name : 'Author',</v>
+        <v>aka : 'aka.',</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>186</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_language : 'Original Language(s)',</v>
+        <v>author_name : 'Author',</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_publication_date : 'Original Publication',</v>
+        <v>original_language : 'Original Language(s)',</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_publisher_name : 'Original Publisher',</v>
+        <v>original_publication_date : 'Original Publication',</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_publication_type : 'Type',</v>
+        <v>original_publisher_name : 'Original Publisher',</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_publication_length : 'Length',</v>
+        <v>original_publication_type : 'Type',</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>writing_period : 'Writing period',</v>
+        <v>original_publication_length : 'Length',</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>editions : 'Editions',</v>
+        <v>writing_period : 'Writing period',</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>edition_title : 'Title',</v>
+        <v>editions : 'Editions',</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>edition_editors : 'Editors',</v>
+        <v>edition_title : 'Title',</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>edition_language : 'Language',</v>
+        <v>edition_editors : 'Editors',</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>isbn : 'ISBN',</v>
+        <v>edition_language : 'Language',</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>27</v>
+        <v>194</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>188</v>
+        <v>84</v>
       </c>
       <c r="E32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>author : 'Author',</v>
+        <v>isbn : 'ISBN',</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>235</v>
+        <v>27</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>original_title : 'Original Title',</v>
+        <v>author : 'Author',</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>language : 'Language',</v>
+        <v>original_title : 'Original Title',</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>editors : 'Editors',</v>
+        <v>language : 'Language',</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>publisher : 'Publisher',</v>
+        <v>editors : 'Editors',</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>binding : 'Binding',</v>
+        <v>publisher : 'Publisher',</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>233</v>
+        <v>199</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>pages : 'pages',</v>
+        <v>binding : 'Binding',</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>publication : 'Published',</v>
+        <v>pages : 'pages',</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>length : 'Length',</v>
+        <v>publication : 'Published',</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>240</v>
+        <v>177</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_header : 'Data Import',</v>
+        <v>length : 'Length',</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>238</v>
       </c>
       <c r="E42" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_type : 'Please select import type',</v>
+        <v>import_header : 'Data Import',</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>238</v>
       </c>
       <c r="E43" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_type_select : 'Import type',</v>
+        <v>import_type : 'Please select import type',</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>238</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_preview_header : 'Preview',</v>
+        <v>import_type_select : 'Import type',</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>238</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_upload_data : 'Upload data',</v>
+        <v>import_preview_header : 'Preview',</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>238</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_preview_label : 'Please change column names using the dropdowns',</v>
+        <v>import_upload_data : 'Upload data',</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>238</v>
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_push_data : 'Push data to database',</v>
+        <v>import_preview_label : 'Please change column names using the dropdowns',</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>238</v>
       </c>
       <c r="E48" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_refresh : 'Refresh',</v>
+        <v>import_push_data : 'Push data to database',</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="E49" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_type_authors : 'Authors',</v>
+        <v>import_refresh : 'Refresh',</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>255</v>
       </c>
       <c r="E50" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_type_texts : 'Texts',</v>
+        <v>import_type_authors : 'Authors',</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>182</v>
+        <v>260</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>255</v>
       </c>
       <c r="E51" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_type_editions : 'Editions',</v>
+        <v>import_type_texts : 'Texts',</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>262</v>
+        <v>182</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>255</v>
       </c>
       <c r="E52" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_error : 'Data has not been imported or the data imported is empty',</v>
+        <v>import_type_editions : 'Editions',</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>255</v>
       </c>
       <c r="E53" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>import_databtn : 'Imported data',</v>
+        <v>import_error : 'Data has not been imported or the data imported is empty',</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>255</v>
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>latest_editsbtn : 'Latest edits',</v>
+        <v>import_databtn : 'Imported data',</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>255</v>
       </c>
       <c r="E55" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>admin_header : 'Admin',</v>
+        <v>latest_editsbtn : 'Latest edits',</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>undoEditBtn : 'Undo all changes',</v>
+        <v>admin_header : 'Admin',</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E57" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>homeBtn : 'Home',</v>
+        <v>undoEditBtn : 'Undo all changes',</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>284</v>
       </c>
       <c r="E58" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>detailedSearchBtn : 'Detailed Search',</v>
+        <v>homeBtn : 'Home',</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>238</v>
+        <v>290</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>284</v>
       </c>
       <c r="E59" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>importDataBtn : 'Import',</v>
+        <v>detailedSearchBtn : 'Detailed Search',</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>284</v>
       </c>
       <c r="E60" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>importDataBtn : 'Import',</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>adminBtn : 'Admin',</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E61" s="1" t="s">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E62" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E63" s="1" t="s">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E64" s="1" t="s">
         <v>280</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed naming of data elements in AuthorTable & TextTable. Added API for texts in AuthorTable
</commit_message>
<xml_diff>
--- a/data/Component_fields.xlsx
+++ b/data/Component_fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarjeisandsnes/lectura/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347951D7-0373-E64B-8BC9-3F61149F35A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC55BE3-D7BC-3149-B0CA-20A36BD0D654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" activeTab="2" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{05B00D71-7402-104C-8673-926CBA0FCBF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Column_list" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="304">
   <si>
     <t>#</t>
   </si>
@@ -238,9 +238,6 @@
     <t>int</t>
   </si>
   <si>
-    <t>nvarchar</t>
-  </si>
-  <si>
     <t>AUTHOR_ID links to separate alternative names table</t>
   </si>
   <si>
@@ -917,13 +914,49 @@
   </si>
   <si>
     <t>worksUnknown</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>identity</t>
+  </si>
+  <si>
+    <t>nvarchar(255)</t>
+  </si>
+  <si>
+    <t>Text original publisher location</t>
+  </si>
+  <si>
+    <t>TEXT_ORIGINAL_PUBLICATION_PUBLISHER_LOC</t>
+  </si>
+  <si>
+    <t>Publisher location</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Text ID</t>
+  </si>
+  <si>
+    <t>EDITION_PUBLICATION_YEAR</t>
+  </si>
+  <si>
+    <t>Publication year of the edition</t>
+  </si>
+  <si>
+    <t>Publication year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -934,6 +967,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -971,7 +1010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -981,11 +1020,39 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1064,15 +1131,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C92C06A-FB8E-9D44-AF23-A294384A6499}" name="Table1" displayName="Table1" ref="A1:F56" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F56" xr:uid="{2C92C06A-FB8E-9D44-AF23-A294384A6499}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A5E7B0C6-2074-3F43-82F5-8187B0E8F44E}" name="#" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{266CDBC5-C85E-8B4C-8E05-3898F7A33CD4}" name="Label" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C52FD609-C89F-3942-896D-6DC79FC67526}" name="SQL name" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{27DED3B4-AC6F-734A-8500-9C1E45380767}" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{8F972DE9-9931-1C42-9EE0-B8076AF4B907}" name="Datatype" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{AD8E2AEE-C3DE-594D-9D4A-21338761046F}" name="Table" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C92C06A-FB8E-9D44-AF23-A294384A6499}" name="Table1" displayName="Table1" ref="A1:I59" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I59" xr:uid="{2C92C06A-FB8E-9D44-AF23-A294384A6499}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Datetime"/>
+        <filter val="identity"/>
+        <filter val="int"/>
+        <filter val="nvarchar(255)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{A5E7B0C6-2074-3F43-82F5-8187B0E8F44E}" name="#" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{266CDBC5-C85E-8B4C-8E05-3898F7A33CD4}" name="Label" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{C52FD609-C89F-3942-896D-6DC79FC67526}" name="SQL name" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{27DED3B4-AC6F-734A-8500-9C1E45380767}" name="Description" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{8F972DE9-9931-1C42-9EE0-B8076AF4B907}" name="Datatype" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{AD8E2AEE-C3DE-594D-9D4A-21338761046F}" name="Table" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{B2B5594E-71DF-C248-BABE-A498513E5934}" name="SQL" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{E97823BD-C6CA-5D45-8C3B-5D06B00D716F}" name="Column1" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{ED7FFC7D-AD97-7E4D-90D9-BDB696089D36}" name="Column2" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1375,13 +1460,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35313EE5-8BCE-A449-9C2B-DB968751C49B}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,7 +1479,7 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1413,8 +1498,17 @@
       <c r="F1" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1425,16 +1519,28 @@
         <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>293</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_ID identity</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_ID': </v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_ID=identity</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1448,13 +1554,25 @@
         <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_NAME nvarchar(255)</v>
+      </c>
+      <c r="H3" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_NAME': </v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_NAME=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1468,13 +1586,25 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_NAME_LANGUAGE nvarchar(255)</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_NAME_LANGUAGE': </v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_NAME_LANGUAGE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1485,7 +1615,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>58</v>
@@ -1493,8 +1623,20 @@
       <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,NA NA</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'NA': </v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>NA=NA</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1505,16 +1647,28 @@
         <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_BIRTH_DATE Datetime</v>
+      </c>
+      <c r="H6" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_BIRTH_DATE': </v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_BIRTH_DATE=Datetime</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1528,13 +1682,25 @@
         <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_BIRTH_CITY nvarchar(255)</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_BIRTH_CITY': </v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_BIRTH_CITY=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1548,13 +1714,25 @@
         <v>42</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_BIRTH_COUNTRY nvarchar(255)</v>
+      </c>
+      <c r="H8" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_BIRTH_COUNTRY': </v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_BIRTH_COUNTRY=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1568,13 +1746,25 @@
         <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_BIRTH_COORDINATES nvarchar(255)</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_BIRTH_COORDINATES': </v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_BIRTH_COORDINATES=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1593,8 +1783,20 @@
       <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_BIRTH_YEAR int</v>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_BIRTH_YEAR': </v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_BIRTH_YEAR=int</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1613,8 +1815,20 @@
       <c r="F11" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_BIRTH_MONTH int</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_BIRTH_MONTH': </v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_BIRTH_MONTH=int</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1633,8 +1847,20 @@
       <c r="F12" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_BIRTH_DAY int</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_BIRTH_DAY': </v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_BIRTH_DAY=int</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1645,16 +1871,28 @@
         <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_DEATH_DATE datetime</v>
+      </c>
+      <c r="H13" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_DEATH_DATE': </v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_DEATH_DATE=datetime</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1665,16 +1903,28 @@
         <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_DEATH_CITY nvarchar(255)</v>
+      </c>
+      <c r="H14" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_DEATH_CITY': </v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_DEATH_CITY=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1685,16 +1935,28 @@
         <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_DEATH_COUNTRY nvarchar(255)</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_DEATH_COUNTRY': </v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_DEATH_COUNTRY=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1705,16 +1967,28 @@
         <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_DEATH_COORDINATES nvarchar(255)</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_DEATH_COORDINATES': </v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_DEATH_COORDINATES=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1725,7 +1999,7 @@
         <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>65</v>
@@ -1733,8 +2007,20 @@
       <c r="F17" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_DEATH_YEAR int</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_DEATH_YEAR': </v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_DEATH_YEAR=int</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1745,7 +2031,7 @@
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>65</v>
@@ -1753,8 +2039,20 @@
       <c r="F18" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_DEATH_MONTH int</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_DEATH_MONTH': </v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_DEATH_MONTH=int</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1765,7 +2063,7 @@
         <v>57</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>65</v>
@@ -1773,8 +2071,20 @@
       <c r="F19" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_DEATH_DAY int</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_DEATH_DAY': </v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_DEATH_DAY=int</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1785,16 +2095,28 @@
         <v>55</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_NATIONALITY nvarchar(255)</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_NATIONALITY': </v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_NATIONALITY=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1813,8 +2135,20 @@
       <c r="F21" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,NA NA</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'NA': </v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>NA=NA</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1833,8 +2167,20 @@
       <c r="F22" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,NA NA</v>
+      </c>
+      <c r="H22" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'NA': </v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>NA=NA</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1853,8 +2199,20 @@
       <c r="F23" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,NA NA</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'NA': </v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>NA=NA</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1873,8 +2231,20 @@
       <c r="F24" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,NA NA</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'NA': </v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>NA=NA</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1885,16 +2255,28 @@
         <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_GENDER nvarchar(255)</v>
+      </c>
+      <c r="H25" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_GENDER': </v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_GENDER=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1902,19 +2284,31 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_FLORUIT nvarchar(255)</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_FLORUIT': </v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_FLORUIT=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1925,7 +2319,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>58</v>
@@ -1933,73 +2327,121 @@
       <c r="F27" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,NA NA</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'NA': </v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>NA=NA</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ID int</v>
+      </c>
+      <c r="H28" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ID': </v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ID=int</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G29" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_TITLE nvarchar(255)</v>
+      </c>
+      <c r="H29" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_TITLE': </v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_TITLE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G30" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_AUTHOR nvarchar(255)</v>
+      </c>
+      <c r="H30" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_AUTHOR': </v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_AUTHOR=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>36</v>
@@ -2011,510 +2453,907 @@
         <v>65</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G31" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_ID int</v>
+      </c>
+      <c r="H31" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_ID': </v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_ID=int</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G32" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_TYPE nvarchar(255)</v>
+      </c>
+      <c r="H32" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_TYPE': </v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_TYPE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G33" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_GENRE nvarchar(255)</v>
+      </c>
+      <c r="H33" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_GENRE': </v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_GENRE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>66</v>
+        <v>294</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G34" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_LANGUAGE nvarchar(255)</v>
+      </c>
+      <c r="H34" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_LANGUAGE': </v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_LANGUAGE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_DATE datetime</v>
+      </c>
+      <c r="H35" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_DATE': </v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_DATE=datetime</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G36" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_YEAR int</v>
+      </c>
+      <c r="H36" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_YEAR': </v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_YEAR=int</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_MONTH int</v>
+      </c>
+      <c r="H37" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_MONTH': </v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_MONTH=int</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="G38" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_DAY int</v>
+      </c>
+      <c r="H38" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_DAY': </v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_DAY=int</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_PUBLISHER nvarchar(255)</v>
+      </c>
+      <c r="H39" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_PUBLISHER': </v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_PUBLISHER=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" s="5" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_PUBLISHER_LOC nvarchar(255)</v>
+      </c>
+      <c r="H40" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_PUBLISHER_LOC': </v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_PUBLISHER_LOC=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G41" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_TYPE nvarchar(255)</v>
+      </c>
+      <c r="H41" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_TYPE': </v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_TYPE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_LENGTH int</v>
+      </c>
+      <c r="H42" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_LENGTH': </v>
+      </c>
+      <c r="I42" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_LENGTH=int</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G43" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ORIGINAL_PUBLICATION_LENGTH_TYPE nvarchar(255)</v>
+      </c>
+      <c r="H43" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ORIGINAL_PUBLICATION_LENGTH_TYPE': </v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ORIGINAL_PUBLICATION_LENGTH_TYPE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_WRITING_START datetime</v>
+      </c>
+      <c r="H44" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_WRITING_START': </v>
+      </c>
+      <c r="I44" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_WRITING_START=datetime</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G45" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_WRITING_END datetime</v>
+      </c>
+      <c r="H45" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_WRITING_END': </v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_WRITING_END=datetime</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G46" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_ID int</v>
+      </c>
+      <c r="H46" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_ID': </v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_ID=int</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G47" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_TITLE nvarchar(255)</v>
+      </c>
+      <c r="H47" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_TITLE': </v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_TITLE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G48" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,AUTHOR_ID int</v>
+      </c>
+      <c r="H48" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'AUTHOR_ID': </v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>AUTHOR_ID=int</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C49" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="D49" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>41</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <v>45</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="F49" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G49" s="5" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,TEXT_ID int</v>
+      </c>
+      <c r="H49" s="5" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'TEXT_ID': </v>
+      </c>
+      <c r="I49" s="5" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>TEXT_ID=int</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>47</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="E50" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G50" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_EDITOR nvarchar(255)</v>
+      </c>
+      <c r="H50" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_EDITOR': </v>
+      </c>
+      <c r="I50" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_EDITOR=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="E51" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G51" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_TRANSLATOR nvarchar(255)</v>
+      </c>
+      <c r="H51" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_TRANSLATOR': </v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_TRANSLATOR=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
-        <v>49</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="E52" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G52" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_PUBLISHER nvarchar(255)</v>
+      </c>
+      <c r="H52" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_PUBLISHER': </v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_PUBLISHER=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="E53" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
-        <v>53</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="G53" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_PUBLICATION_DATE datetime</v>
+      </c>
+      <c r="H53" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_PUBLICATION_DATE': </v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_PUBLICATION_DATE=datetime</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>196</v>
+        <v>303</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>208</v>
+        <v>301</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>219</v>
+        <v>302</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+      <c r="G54" s="5" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_PUBLICATION_YEAR int</v>
+      </c>
+      <c r="H54" s="5" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_PUBLICATION_YEAR': </v>
+      </c>
+      <c r="I54" s="5" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_PUBLICATION_YEAR=int</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
+        <v>51</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G55" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_ISBN nvarchar(255)</v>
+      </c>
+      <c r="H55" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_ISBN': </v>
+      </c>
+      <c r="I55" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_ISBN=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>52</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G56" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_ISBN13 nvarchar(255)</v>
+      </c>
+      <c r="H56" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_ISBN13': </v>
+      </c>
+      <c r="I56" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_ISBN13=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>53</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G57" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_LENGTH int</v>
+      </c>
+      <c r="H57" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_LENGTH': </v>
+      </c>
+      <c r="I57" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_LENGTH=int</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G58" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_LANGUAGE nvarchar(255)</v>
+      </c>
+      <c r="H58" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_LANGUAGE': </v>
+      </c>
+      <c r="I58" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_LANGUAGE=nvarchar(255)</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>55</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>188</v>
+      <c r="E59" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G59" s="1" t="str">
+        <f>_xlfn.CONCAT(",",Table1[[#This Row],[SQL name]]," ",Table1[[#This Row],[Datatype]])</f>
+        <v>,EDITION_BINDING nvarchar(255)</v>
+      </c>
+      <c r="H59" s="1" t="str">
+        <f>_xlfn.CONCAT("'",Table1[[#This Row],[SQL name]],"': ")</f>
+        <v xml:space="preserve">'EDITION_BINDING': </v>
+      </c>
+      <c r="I59" s="1" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[SQL name]],"=",Table1[[#This Row],[Datatype]])</f>
+        <v>EDITION_BINDING=nvarchar(255)</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2542,70 +3381,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2617,8 +3456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298DE665-662E-684B-8509-C9EC46F060F1}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E64"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2631,7 +3470,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2640,15 +3479,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>27</v>
@@ -2660,10 +3499,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -2675,7 +3514,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -2690,7 +3529,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
@@ -2705,10 +3544,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
@@ -2720,10 +3559,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
@@ -2735,10 +3574,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
@@ -2750,39 +3589,40 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E9:E10" si="1">_xlfn.CONCAT("",B9," : '",C9,"',")</f>
         <v>influence : 'Influences:',</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>255</v>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>influenced : 'Influenced:',</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>27</v>
@@ -2794,10 +3634,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -2809,10 +3649,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>27</v>
@@ -2824,10 +3664,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>27</v>
@@ -2839,40 +3679,40 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f t="shared" ref="E15:E16" si="1">_xlfn.CONCAT("",B15," : '",C15,"',")</f>
+        <f t="shared" ref="E15:E16" si="2">_xlfn.CONCAT("",B15," : '",C15,"',")</f>
         <v>edit_country_birth_description : ' (city, country) of birth',</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="D16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>edit_country_death_description : ' (city, country) of death',</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>27</v>
@@ -2884,10 +3724,10 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>27</v>
@@ -2899,10 +3739,10 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>27</v>
@@ -2914,13 +3754,13 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2929,13 +3769,13 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2944,13 +3784,13 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2959,13 +3799,13 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2974,13 +3814,13 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2989,13 +3829,13 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3004,13 +3844,13 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3019,13 +3859,13 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3034,13 +3874,13 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3049,13 +3889,13 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3064,13 +3904,13 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3079,13 +3919,13 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3094,13 +3934,13 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3109,13 +3949,13 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3124,13 +3964,13 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3139,13 +3979,13 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3154,13 +3994,13 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3169,13 +4009,13 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3184,13 +4024,13 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3199,13 +4039,13 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3214,13 +4054,13 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3229,13 +4069,13 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3244,13 +4084,13 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3259,13 +4099,13 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E43" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3274,13 +4114,13 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3289,13 +4129,13 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3304,13 +4144,13 @@
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="D46" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3319,13 +4159,13 @@
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3334,13 +4174,13 @@
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>252</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E48" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3349,13 +4189,13 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="D49" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E49" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3364,13 +4204,13 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E50" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3379,13 +4219,13 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E51" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3394,13 +4234,13 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E52" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3409,13 +4249,13 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>262</v>
-      </c>
       <c r="D53" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E53" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3424,13 +4264,13 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3439,13 +4279,13 @@
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E55" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3454,13 +4294,13 @@
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3469,13 +4309,13 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E57" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3484,13 +4324,13 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E58" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3499,13 +4339,13 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E59" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3514,13 +4354,13 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E60" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3529,13 +4369,13 @@
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E61" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3544,12 +4384,12 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E62" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E64" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>